<commit_message>
changes pushed on 01 Jan 18
</commit_message>
<xml_diff>
--- a/Meeting Agenda_Sheet.xlsx
+++ b/Meeting Agenda_Sheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\Herewego App\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mydeen\Mcube_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Agenda" sheetId="1" r:id="rId1"/>
@@ -670,8 +670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,8 +813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>